<commit_message>
Updated with CWF entries
</commit_message>
<xml_diff>
--- a/PPV/MCChecker/##Name##_##w##_##LABEL##_PPV_Unit_Overview.xlsx
+++ b/PPV/MCChecker/##Name##_##w##_##LABEL##_PPV_Unit_Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\PPV\MCChecker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\Automation\PPV\MCChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B550BA2-9DA3-464B-842D-F75A0F466E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550E37BA-658E-4113-9CD7-14949D5D52EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B533D783-8E94-47EE-A5E0-31DB8C66C10E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B533D783-8E94-47EE-A5E0-31DB8C66C10E}"/>
   </bookViews>
   <sheets>
     <sheet name="CHA" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
   <si>
     <t>Unit</t>
   </si>
@@ -485,6 +485,12 @@
   </si>
   <si>
     <t>REGISTERS</t>
+  </si>
+  <si>
+    <t>Show Top</t>
+  </si>
+  <si>
+    <t>ShowTop</t>
   </si>
 </sst>
 </file>
@@ -1443,15 +1449,6 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1466,6 +1463,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2774,6 +2780,16 @@
 </table>
 </file>
 
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FB1EAA75-A4FE-4344-86D9-B9C04E12A825}" name="showtop" displayName="showtop" ref="D7:D10" totalsRowShown="0">
+  <autoFilter ref="D7:D10" xr:uid="{FB1EAA75-A4FE-4344-86D9-B9C04E12A825}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{349EF60A-141C-4C7E-825C-1F1F5680C9A6}" name="ShowTop"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3587,8 +3603,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AM59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3711,20 +3727,24 @@
       <c r="U2" s="87"/>
       <c r="V2" s="87"/>
       <c r="W2" s="87"/>
-      <c r="X2" s="105" t="s">
+      <c r="X2" s="102" t="s">
         <v>136</v>
       </c>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="106"/>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="108" t="s">
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="104"/>
+      <c r="AB2" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="AC2" s="109"/>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
-      <c r="AF2" s="87"/>
-      <c r="AG2" s="87"/>
+      <c r="AC2" s="106"/>
+      <c r="AD2" s="102" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE2" s="103"/>
+      <c r="AF2" s="103"/>
+      <c r="AG2" s="67">
+        <v>1</v>
+      </c>
       <c r="AH2" s="87"/>
       <c r="AI2" s="87"/>
       <c r="AJ2" s="87"/>
@@ -3984,11 +4004,11 @@
       </c>
       <c r="AB5" s="75"/>
       <c r="AC5" s="82" t="str" cm="1">
-        <f t="array" ref="AC5">IFERROR("CORE"&amp;_xlfn._xlws.FILTER(misc[location],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-1,1)),"")</f>
+        <f t="array" ref="AC5">IFERROR("CORE"&amp;_xlfn._xlws.FILTER(misc[location],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-AG2,1)),"")</f>
         <v>CORE8</v>
       </c>
       <c r="AD5" s="79" cm="1">
-        <f t="array" ref="AD5">IFERROR(_xlfn._xlws.FILTER(misc[Core_Hitter_Count],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-1,1)),"")</f>
+        <f t="array" ref="AD5">IFERROR(_xlfn._xlws.FILTER(misc[Core_Hitter_Count],misc[Core_Hitter_Count]&gt;=MAX(misc[Core_Hitter_Count]-$AG$2,1)),"")</f>
         <v>1</v>
       </c>
       <c r="AE5" s="89" t="str" cm="1">
@@ -3997,20 +4017,20 @@
       </c>
       <c r="AF5" s="69"/>
       <c r="AG5" s="88" t="str" cm="1">
-        <f t="array" ref="AG5">IFERROR("CHA"&amp;_xlfn._xlws.FILTER(misc[location],misc[CHA_Hitter_Count]&gt;=MAX(misc[CHA_Hitter_Count]-1,1)),"")</f>
+        <f t="array" ref="AG5">IFERROR("CHA"&amp;_xlfn._xlws.FILTER(misc[location],misc[CHA_Hitter_Count]&gt;=MAX(misc[CHA_Hitter_Count]-$AG$2,1)),"")</f>
         <v/>
       </c>
       <c r="AH5" s="79" t="str" cm="1">
-        <f t="array" ref="AH5">IFERROR(_xlfn._xlws.FILTER(misc[CHA_Hitter_Count],misc[CHA_Hitter_Count]&gt;=MAX(misc[CHA_Hitter_Count]-1,1)),"")</f>
+        <f t="array" ref="AH5">IFERROR(_xlfn._xlws.FILTER(misc[CHA_Hitter_Count],misc[CHA_Hitter_Count]&gt;=MAX(misc[CHA_Hitter_Count]-$AG$2,1)),"")</f>
         <v/>
       </c>
       <c r="AI5" s="69"/>
       <c r="AJ5" s="88" t="str" cm="1">
-        <f t="array" ref="AJ5">IFERROR("LLC"&amp;_xlfn._xlws.FILTER(misc[location],misc[LLC_Hitter_Count]&gt;=MAX(misc[LLC_Hitter_Count]-1,1)),"")</f>
+        <f t="array" ref="AJ5">IFERROR("LLC"&amp;_xlfn._xlws.FILTER(misc[location],misc[LLC_Hitter_Count]&gt;=MAX(misc[LLC_Hitter_Count]-$AG$2,1)),"")</f>
         <v/>
       </c>
       <c r="AK5" s="79" t="str" cm="1">
-        <f t="array" ref="AK5">IFERROR(_xlfn._xlws.FILTER(misc[LLC_Hitter_Count],misc[LLC_Hitter_Count]&gt;=MAX(misc[LLC_Hitter_Count]-1,1)),"")</f>
+        <f t="array" ref="AK5">IFERROR(_xlfn._xlws.FILTER(misc[LLC_Hitter_Count],misc[LLC_Hitter_Count]&gt;=MAX(misc[LLC_Hitter_Count]-$AG$2,1)),"")</f>
         <v/>
       </c>
       <c r="AL5" s="87"/>
@@ -6930,7 +6950,7 @@
       <c r="A59" s="87"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="L1:AK1"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
@@ -6940,6 +6960,7 @@
     <mergeCell ref="Z3:AA3"/>
     <mergeCell ref="X2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
   </mergeCells>
   <conditionalFormatting sqref="X5:X10">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
@@ -7095,12 +7116,18 @@
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{56C41764-2A11-4836-9359-58EBFBEBEAB9}">
           <x14:formula1>
             <xm:f>ErrorData!$D$3:$D$4</xm:f>
           </x14:formula1>
           <xm:sqref>AB2:AC2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3544B18A-8CCB-49A3-BFE4-1623780809C8}">
+          <x14:formula1>
+            <xm:f>_xlfn._TRO_TRAILING(ErrorData!$D$8:$D$12)</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7112,15 +7139,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEF356-01A3-45DB-BFFF-83FE6984CD58}">
   <dimension ref="A1:AP182"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AO5" sqref="AO5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="76.33203125" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="65.77734375" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
     <col min="11" max="11" width="70.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="72.6640625" bestFit="1" customWidth="1"/>
@@ -7149,11 +7176,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="107" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="104"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="109"/>
       <c r="F1" t="s">
         <v>135</v>
       </c>
@@ -7774,6 +7801,9 @@
       </c>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>141</v>
+      </c>
       <c r="F7">
         <v>0</v>
       </c>
@@ -7894,6 +7924,9 @@
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="F8">
         <v>0</v>
       </c>
@@ -7992,6 +8025,9 @@
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="F9">
         <v>0</v>
       </c>
@@ -8090,6 +8126,9 @@
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>3</v>
+      </c>
       <c r="F10">
         <v>0</v>
       </c>
@@ -21479,12 +21518,13 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>